<commit_message>
created gerbers for sensor board, and made headway on the BOM.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donald.dunn\Documents\School\Win_18\ENEL 400\AlbatrossHardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob Dunn\Documents\School\Win_18\ENEL 400\AlbatrossHardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00478E1-C30A-4067-A517-69DBC03E4EE8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02519DBD-F163-4397-A346-88C93AAFAC49}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{1D1281EF-6FB3-4329-9A38-48FD45BC2E20}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="69">
   <si>
     <t>Part Number</t>
   </si>
@@ -42,9 +42,6 @@
     <t>MCP6001UT-I/OTTR-ND</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Cost (each)</t>
   </si>
   <si>
@@ -58,13 +55,190 @@
   </si>
   <si>
     <t>DZ2W03300LCT-ND</t>
+  </si>
+  <si>
+    <t>Orange LED</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>GRN LED</t>
+  </si>
+  <si>
+    <t>OR resistor</t>
+  </si>
+  <si>
+    <t>1uF capacitor</t>
+  </si>
+  <si>
+    <t>0.1uF capacitor</t>
+  </si>
+  <si>
+    <t>160-1445-1-nd</t>
+  </si>
+  <si>
+    <t>160-1447-1-nd</t>
+  </si>
+  <si>
+    <t>160-1828-1-nd</t>
+  </si>
+  <si>
+    <t>2.54mm Jumper</t>
+  </si>
+  <si>
+    <t>WM23943-ND</t>
+  </si>
+  <si>
+    <t># ordered</t>
+  </si>
+  <si>
+    <t># needed</t>
+  </si>
+  <si>
+    <t>BLU LED</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>30pF capacitor</t>
+  </si>
+  <si>
+    <t>0.33uF Capacitor</t>
+  </si>
+  <si>
+    <t>8mHz Crystal</t>
+  </si>
+  <si>
+    <t>molex 3x2 micro jack</t>
+  </si>
+  <si>
+    <t>molex 3x2 micro plug</t>
+  </si>
+  <si>
+    <t>sheilded wire</t>
+  </si>
+  <si>
+    <t>2pin Screw term</t>
+  </si>
+  <si>
+    <t>1297-1108-1-ND</t>
+  </si>
+  <si>
+    <t>1297-1112-2-ND</t>
+  </si>
+  <si>
+    <t>6pos screw term</t>
+  </si>
+  <si>
+    <t>4pin vertical 2.54 head</t>
+  </si>
+  <si>
+    <t>2.54mm 2pin male head</t>
+  </si>
+  <si>
+    <t>buzzer threw hole</t>
+  </si>
+  <si>
+    <t>buzzer wired</t>
+  </si>
+  <si>
+    <t>10k 5turn pot</t>
+  </si>
+  <si>
+    <t>3214X-1-103ECT-ND</t>
+  </si>
+  <si>
+    <t>10R pot</t>
+  </si>
+  <si>
+    <t>3314G-1-100ECT-ND</t>
+  </si>
+  <si>
+    <t>10uF Cap</t>
+  </si>
+  <si>
+    <t>2.2uF Cap</t>
+  </si>
+  <si>
+    <t>reset switch</t>
+  </si>
+  <si>
+    <t>CKN9085CT-ND</t>
+  </si>
+  <si>
+    <t>3.3 500mA LDO</t>
+  </si>
+  <si>
+    <t>296-13424-1-ND</t>
+  </si>
+  <si>
+    <t>1 amp 5V buck</t>
+  </si>
+  <si>
+    <t>9V battery clip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9V battery </t>
+  </si>
+  <si>
+    <t>bluetooth module</t>
+  </si>
+  <si>
+    <t>stm32f4 MCU</t>
+  </si>
+  <si>
+    <t>497-17437-1-nd</t>
+  </si>
+  <si>
+    <t>631-1100-nd</t>
+  </si>
+  <si>
+    <t>sam1093-36-nd</t>
+  </si>
+  <si>
+    <t>wm1815-nd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none </t>
+  </si>
+  <si>
+    <t>10 (just in case)</t>
+  </si>
+  <si>
+    <t>10pin Male Head</t>
+  </si>
+  <si>
+    <t>SAM8796-ND</t>
+  </si>
+  <si>
+    <t>945-2201-ND</t>
+  </si>
+  <si>
+    <t>molex micro crimp fem</t>
+  </si>
+  <si>
+    <t>wm1837ct-ND</t>
+  </si>
+  <si>
+    <t>RN4871-I/RM128-ND</t>
+  </si>
+  <si>
+    <t>arden</t>
+  </si>
+  <si>
+    <t>rob</t>
+  </si>
+  <si>
+    <t>Not needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +251,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,9 +286,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,21 +609,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD06ABFE-BDAD-4DD9-8C2C-79FF4F2D0F41}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U12:U13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -441,43 +635,782 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2">
         <v>0.37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
-        <v>0.48</v>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>67</v>
+      </c>
+      <c r="F38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F42" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated resistors and capacitors in BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob Dunn\Documents\School\Win_18\ENEL 400\AlbatrossHardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aoh30\Desktop\400\AlbatrossHardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02519DBD-F163-4397-A346-88C93AAFAC49}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{1D1281EF-6FB3-4329-9A38-48FD45BC2E20}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="109">
   <si>
     <t>Part Number</t>
   </si>
@@ -232,13 +231,133 @@
   </si>
   <si>
     <t>Not needed</t>
+  </si>
+  <si>
+    <t>2R</t>
+  </si>
+  <si>
+    <t>CR1,CR6,CR9,CR10,CR11,CR15,CR16,CR17,SR1,SR2,SR5,SR6</t>
+  </si>
+  <si>
+    <t>RR08P10.0KDCT-ND</t>
+  </si>
+  <si>
+    <t>330R</t>
+  </si>
+  <si>
+    <t>CR2,CR4,CR5,CR7,CR8,CR12,CR13,CR14,CR18,CR19,CR20,CR21,CR22,CR23,CR24,CR25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 311-330HRCT-ND</t>
+  </si>
+  <si>
+    <t>311-0.0GRCT-ND</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>4K7</t>
+  </si>
+  <si>
+    <t>CR3</t>
+  </si>
+  <si>
+    <t>311-4.70KHRCT-ND</t>
+  </si>
+  <si>
+    <t>150R</t>
+  </si>
+  <si>
+    <t>500R</t>
+  </si>
+  <si>
+    <t>30K</t>
+  </si>
+  <si>
+    <t>100R</t>
+  </si>
+  <si>
+    <t>SR10,SR11</t>
+  </si>
+  <si>
+    <t>SR12</t>
+  </si>
+  <si>
+    <t>SR3</t>
+  </si>
+  <si>
+    <t>SR7</t>
+  </si>
+  <si>
+    <t>SR8</t>
+  </si>
+  <si>
+    <t>RR08P150DCT-ND</t>
+  </si>
+  <si>
+    <t>541-3301-1-ND</t>
+  </si>
+  <si>
+    <t>499R</t>
+  </si>
+  <si>
+    <t>311-499HRCT-ND</t>
+  </si>
+  <si>
+    <t>311-2.00HRCT-ND</t>
+  </si>
+  <si>
+    <t>311-100HRCT-ND</t>
+  </si>
+  <si>
+    <t>RR08P30.0KDCT-ND</t>
+  </si>
+  <si>
+    <t>SC1,SC2,CC19</t>
+  </si>
+  <si>
+    <t>CC18</t>
+  </si>
+  <si>
+    <t>SC3,SC4,CC1,CC2,CC3,CC4,CC5,CC6,CC7,CC8,CC9,CC14,CC17</t>
+  </si>
+  <si>
+    <t>CC10,CC11</t>
+  </si>
+  <si>
+    <t>CC16</t>
+  </si>
+  <si>
+    <t>CC12,CC13</t>
+  </si>
+  <si>
+    <t>587-1256-1-ND</t>
+  </si>
+  <si>
+    <t>587-1242-1-ND</t>
+  </si>
+  <si>
+    <t>399-1095-1-ND</t>
+  </si>
+  <si>
+    <t>490-1414-1-ND</t>
+  </si>
+  <si>
+    <t>399-4917-1-ND</t>
+  </si>
+  <si>
+    <t>587-1430-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500R Cost a lot so I looked up a 499R for much cheaper </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,13 +384,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -286,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -295,6 +440,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,23 +766,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD06ABFE-BDAD-4DD9-8C2C-79FF4F2D0F41}">
-  <dimension ref="A1:F42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" customWidth="1"/>
+    <col min="1" max="1" width="23.46484375" customWidth="1"/>
+    <col min="2" max="2" width="21.46484375" customWidth="1"/>
+    <col min="3" max="3" width="21.53125" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -644,7 +802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -664,7 +822,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -684,7 +842,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -704,7 +862,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -724,7 +882,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -744,7 +902,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -764,7 +922,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -784,7 +942,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -804,7 +962,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -824,7 +982,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -844,7 +1002,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -864,7 +1022,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -884,7 +1042,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -904,7 +1062,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -924,7 +1082,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -944,7 +1102,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -964,7 +1122,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -984,7 +1142,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1004,7 +1162,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1024,7 +1182,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -1044,7 +1202,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1061,7 +1219,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1081,7 +1239,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1101,7 +1259,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1121,7 +1279,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1141,7 +1299,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1161,7 +1319,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1172,7 +1330,7 @@
         <v>40</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E28" t="s">
         <v>67</v>
@@ -1181,7 +1339,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1192,7 +1350,7 @@
         <v>42</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E29" t="s">
         <v>67</v>
@@ -1201,7 +1359,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -1221,85 +1379,85 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" t="s">
-        <v>66</v>
+        <v>96</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
         <v>67</v>
       </c>
-      <c r="F33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F33">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" t="s">
-        <v>66</v>
+        <v>97</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
       </c>
       <c r="E34" t="s">
         <v>67</v>
       </c>
-      <c r="F34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F34">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="47.55" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" t="s">
-        <v>66</v>
+        <v>98</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="D35">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E35" t="s">
         <v>67</v>
       </c>
-      <c r="F35" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F35">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" t="s">
-        <v>66</v>
+        <v>99</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -1307,19 +1465,19 @@
       <c r="E36" t="s">
         <v>67</v>
       </c>
-      <c r="F36" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F36">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" t="s">
-        <v>66</v>
+        <v>100</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1327,19 +1485,19 @@
       <c r="E37" t="s">
         <v>67</v>
       </c>
-      <c r="F37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F37">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" t="s">
-        <v>66</v>
+        <v>101</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="D38">
         <v>2</v>
@@ -1347,15 +1505,15 @@
       <c r="E38" t="s">
         <v>67</v>
       </c>
-      <c r="F38" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F38">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B39" t="s">
         <v>66</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E39" t="s">
@@ -1365,11 +1523,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B40" t="s">
         <v>66</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E40" t="s">
@@ -1379,29 +1537,32 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
-      </c>
-      <c r="F41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+      <c r="D41">
+        <v>24</v>
+      </c>
+      <c r="F41">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" t="s">
-        <v>66</v>
+        <v>76</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D42" t="s">
         <v>58</v>
@@ -1409,9 +1570,157 @@
       <c r="E42" t="s">
         <v>59</v>
       </c>
-      <c r="F42" t="s">
-        <v>66</v>
-      </c>
+      <c r="F42">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43">
+        <v>16</v>
+      </c>
+      <c r="E43" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="7">
+        <v>4</v>
+      </c>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7">
+        <v>4.6399999999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" s="7">
+        <v>4</v>
+      </c>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added pdf of bom with nice tables.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donald.dunn\Documents\School\Win_18\ENEL 400\AlbatrossHardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9F3B45-DD68-4C06-8012-EB22BD635120}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F739BC-22CA-403B-835B-4836EFB1FC77}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="114">
   <si>
     <t>Part Number</t>
   </si>
@@ -367,9 +367,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sum = </t>
-  </si>
-  <si>
-    <t>ish</t>
   </si>
 </sst>
 </file>
@@ -481,6 +478,32 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3124FECC-685F-44ED-89EB-7BB8EC99C60E}" name="Table2" displayName="Table2" ref="A1:C45" totalsRowShown="0">
+  <autoFilter ref="A1:C45" xr:uid="{26B14785-F214-412C-B38B-156AC59956A2}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{1985A9EF-31F9-41CF-A274-0B3CC20EF885}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{FDABFAB7-B05C-4824-AE4F-7A63FD8E1B2E}" name="Board Referances"/>
+    <tableColumn id="3" xr3:uid="{87EC0948-013D-4678-BE41-F392549DECFF}" name="Part Number"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{23991475-40B1-4CAF-90D7-8B2C9B8BC9AA}" name="Table4" displayName="Table4" ref="E1:I49" totalsRowShown="0">
+  <autoFilter ref="E1:I49" xr:uid="{6DADFDAD-0593-4B9A-BB61-05154921BBFB}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{99B432BE-09FD-4E1A-8A62-478D991540D5}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0948B9F9-0483-4286-B335-DDDCF59F86F4}" name="# needed"/>
+    <tableColumn id="3" xr3:uid="{53B9CA62-8B6D-4EB1-8B66-2B27D2AB4702}" name="# ordered"/>
+    <tableColumn id="4" xr3:uid="{35768FE5-BB6C-4211-94C1-3C29340F95C8}" name="Cost (each)"/>
+    <tableColumn id="5" xr3:uid="{392B18CD-D73E-42F9-99E8-844392EB4C4F}" name="Extended"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -782,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +815,11 @@
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -805,16 +832,19 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>110</v>
       </c>
     </row>
@@ -828,17 +858,20 @@
       <c r="C2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D2">
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>8</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>15</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>0.37</v>
       </c>
-      <c r="G2">
-        <f xml:space="preserve"> E2*F2</f>
+      <c r="I2">
+        <f xml:space="preserve"> G2*H2</f>
         <v>5.55</v>
       </c>
     </row>
@@ -852,17 +885,20 @@
       <c r="C3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D3">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>14</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>0.39700000000000002</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G49" si="0" xml:space="preserve"> E3*F3</f>
+      <c r="I3">
+        <f t="shared" ref="I3:I30" si="0" xml:space="preserve"> G3*H3</f>
         <v>5.5579999999999998</v>
       </c>
     </row>
@@ -876,16 +912,19 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>6</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>0.48</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <f t="shared" si="0"/>
         <v>2.88</v>
       </c>
@@ -901,16 +940,19 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
         <v>7</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>10</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>0.20200000000000001</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <f t="shared" si="0"/>
         <v>2.02</v>
       </c>
@@ -925,16 +967,19 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6">
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>0.218</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <f t="shared" si="0"/>
         <v>2.1800000000000002</v>
       </c>
@@ -949,16 +994,19 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7">
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7">
         <v>4</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>7</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>0.43</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <f t="shared" si="0"/>
         <v>3.01</v>
       </c>
@@ -974,16 +1022,19 @@
       <c r="C8" t="s">
         <v>99</v>
       </c>
-      <c r="D8">
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8">
         <v>1</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>5</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>0.49</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <f t="shared" si="0"/>
         <v>2.4500000000000002</v>
       </c>
@@ -998,16 +1049,19 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9">
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9">
         <v>6</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>8</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <f t="shared" si="0"/>
         <v>4.6399999999999997</v>
       </c>
@@ -1022,16 +1076,19 @@
       <c r="C10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D10">
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
         <v>6</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>10</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>0.379</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <f t="shared" si="0"/>
         <v>3.79</v>
       </c>
@@ -1046,16 +1103,19 @@
       <c r="C11" t="s">
         <v>43</v>
       </c>
-      <c r="D11">
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11">
         <v>2</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>4</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>0.25</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1070,16 +1130,19 @@
       <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="D12">
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12">
         <v>3</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>3</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>0.66</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <f t="shared" si="0"/>
         <v>1.98</v>
       </c>
@@ -1094,16 +1157,19 @@
       <c r="C13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D13">
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13">
         <v>1</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>3.58</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <f t="shared" si="0"/>
         <v>3.58</v>
       </c>
@@ -1118,16 +1184,19 @@
       <c r="C14" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D14">
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14">
         <v>1</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>3</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>0.89</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <f t="shared" si="0"/>
         <v>2.67</v>
       </c>
@@ -1142,16 +1211,19 @@
       <c r="C15" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D15">
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15">
         <v>1</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>3</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>2.06</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <f t="shared" si="0"/>
         <v>6.18</v>
       </c>
@@ -1166,22 +1238,24 @@
       <c r="C16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D16">
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16">
         <v>2</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>2</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>10.9</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <f t="shared" si="0"/>
         <v>21.8</v>
       </c>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1191,21 +1265,24 @@
       <c r="C17" t="s">
         <v>51</v>
       </c>
-      <c r="D17">
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17">
         <v>1</v>
       </c>
-      <c r="E17">
+      <c r="G17">
         <v>1</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>14.61</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <f t="shared" si="0"/>
         <v>14.61</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1215,21 +1292,24 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D18">
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18">
         <v>1</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <v>2</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>0.39</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1239,21 +1319,24 @@
       <c r="C19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D19">
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19">
         <v>8</v>
       </c>
-      <c r="E19">
+      <c r="G19">
         <v>10</v>
       </c>
-      <c r="F19">
+      <c r="H19">
         <v>0.54</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1263,21 +1346,24 @@
       <c r="C20" t="s">
         <v>53</v>
       </c>
-      <c r="D20">
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20">
         <v>8</v>
       </c>
-      <c r="E20">
+      <c r="G20">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="H20">
         <v>1.599</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <f t="shared" si="0"/>
         <v>15.99</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1287,21 +1373,24 @@
       <c r="C21" t="s">
         <v>59</v>
       </c>
-      <c r="D21">
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21">
         <v>25</v>
       </c>
-      <c r="E21">
+      <c r="G21">
         <v>10</v>
       </c>
-      <c r="F21">
+      <c r="H21">
         <v>0.14899999999999999</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <f t="shared" si="0"/>
         <v>1.49</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1311,18 +1400,21 @@
       <c r="C22" t="s">
         <v>69</v>
       </c>
-      <c r="E22">
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22">
         <v>0</v>
       </c>
-      <c r="F22">
+      <c r="H22">
         <v>0</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1332,21 +1424,24 @@
       <c r="C23" t="s">
         <v>30</v>
       </c>
-      <c r="D23">
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23">
         <v>1</v>
       </c>
-      <c r="E23">
+      <c r="G23">
         <v>2</v>
       </c>
-      <c r="F23">
+      <c r="H23">
         <v>3.83</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <f t="shared" si="0"/>
         <v>7.66</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1356,21 +1451,24 @@
       <c r="C24" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D24">
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24">
         <v>4</v>
       </c>
-      <c r="E24">
+      <c r="G24">
         <v>5</v>
       </c>
-      <c r="F24">
+      <c r="H24">
         <v>8.91</v>
       </c>
-      <c r="G24">
+      <c r="I24">
         <f t="shared" si="0"/>
         <v>44.55</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1380,21 +1478,24 @@
       <c r="C25" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D25">
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25">
         <v>14</v>
       </c>
-      <c r="E25">
+      <c r="G25">
         <v>15</v>
       </c>
-      <c r="F25">
+      <c r="H25">
         <v>0.437</v>
       </c>
-      <c r="G25">
+      <c r="I25">
         <f t="shared" si="0"/>
         <v>6.5549999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1404,21 +1505,24 @@
       <c r="C26" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D26">
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26">
         <v>4</v>
       </c>
-      <c r="E26">
+      <c r="G26">
         <v>5</v>
       </c>
-      <c r="F26">
+      <c r="H26">
         <v>3.9</v>
       </c>
-      <c r="G26">
+      <c r="I26">
         <f t="shared" si="0"/>
         <v>19.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1428,21 +1532,24 @@
       <c r="C27" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D27">
+      <c r="E27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27">
         <v>4</v>
       </c>
-      <c r="E27">
+      <c r="G27">
         <v>5</v>
       </c>
-      <c r="F27">
+      <c r="H27">
         <v>2.91</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <f t="shared" si="0"/>
         <v>14.55</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1452,21 +1559,24 @@
       <c r="C28" t="s">
         <v>37</v>
       </c>
-      <c r="D28">
+      <c r="E28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28">
         <v>4</v>
       </c>
-      <c r="E28">
+      <c r="G28">
         <v>5</v>
       </c>
-      <c r="F28">
+      <c r="H28">
         <v>3.55</v>
       </c>
-      <c r="G28">
+      <c r="I28">
         <f t="shared" si="0"/>
         <v>17.75</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1476,21 +1586,24 @@
       <c r="C29" t="s">
         <v>39</v>
       </c>
-      <c r="D29">
+      <c r="E29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29">
         <v>4</v>
       </c>
-      <c r="E29">
+      <c r="G29">
         <v>5</v>
       </c>
-      <c r="F29">
+      <c r="H29">
         <v>2.4</v>
       </c>
-      <c r="G29">
+      <c r="I29">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1500,21 +1613,24 @@
       <c r="C30" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D30">
+      <c r="E30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30">
         <v>1</v>
       </c>
-      <c r="E30">
+      <c r="G30">
         <v>2</v>
       </c>
-      <c r="F30">
+      <c r="H30">
         <v>2.99</v>
       </c>
-      <c r="G30">
+      <c r="I30">
         <f t="shared" si="0"/>
         <v>5.98</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -1524,21 +1640,24 @@
       <c r="C31" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D31">
+      <c r="E31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31">
         <v>9</v>
       </c>
-      <c r="E31">
+      <c r="G31">
         <v>15</v>
       </c>
-      <c r="F31">
+      <c r="H31">
         <v>0.159</v>
       </c>
-      <c r="G31">
-        <f xml:space="preserve"> E31*F31</f>
+      <c r="I31">
+        <f t="shared" ref="I31:I45" si="1" xml:space="preserve"> G31*H31</f>
         <v>2.3850000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1548,21 +1667,24 @@
       <c r="C32" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D32">
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32">
         <v>1</v>
       </c>
-      <c r="E32">
+      <c r="G32">
         <v>10</v>
       </c>
-      <c r="F32">
+      <c r="H32">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="G32">
-        <f xml:space="preserve"> E32*F32</f>
+      <c r="I32">
+        <f t="shared" si="1"/>
         <v>0.74</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1572,21 +1694,24 @@
       <c r="C33" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D33">
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33">
         <v>19</v>
       </c>
-      <c r="E33">
+      <c r="G33">
         <v>30</v>
       </c>
-      <c r="F33">
+      <c r="H33">
         <v>0.03</v>
       </c>
-      <c r="G33">
-        <f xml:space="preserve"> E33*F33</f>
+      <c r="I33">
+        <f t="shared" si="1"/>
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -1596,21 +1721,24 @@
       <c r="C34" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D34">
+      <c r="E34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34">
         <v>2</v>
       </c>
-      <c r="E34">
+      <c r="G34">
         <v>10</v>
       </c>
-      <c r="F34">
+      <c r="H34">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="G34">
-        <f xml:space="preserve"> E34*F34</f>
+      <c r="I34">
+        <f t="shared" si="1"/>
         <v>0.84000000000000008</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -1620,21 +1748,24 @@
       <c r="C35" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D35">
+      <c r="E35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35">
         <v>1</v>
       </c>
-      <c r="E35">
+      <c r="G35">
         <v>10</v>
       </c>
-      <c r="F35">
+      <c r="H35">
         <v>0.10199999999999999</v>
       </c>
-      <c r="G35">
-        <f xml:space="preserve"> E35*F35</f>
+      <c r="I35">
+        <f t="shared" si="1"/>
         <v>1.02</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1644,21 +1775,24 @@
       <c r="C36" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D36">
+      <c r="E36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36">
         <v>2</v>
       </c>
-      <c r="E36">
+      <c r="G36">
         <v>10</v>
       </c>
-      <c r="F36">
+      <c r="H36">
         <v>0.122</v>
       </c>
-      <c r="G36">
-        <f xml:space="preserve"> E36*F36</f>
+      <c r="I36">
+        <f t="shared" si="1"/>
         <v>1.22</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -1668,21 +1802,24 @@
       <c r="C37" t="s">
         <v>64</v>
       </c>
-      <c r="D37">
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37">
         <v>24</v>
       </c>
-      <c r="E37">
+      <c r="G37">
         <v>100</v>
       </c>
-      <c r="F37">
+      <c r="H37">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="G37">
-        <f xml:space="preserve"> E37*F37</f>
+      <c r="I37">
+        <f t="shared" si="1"/>
         <v>4.1000000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -1692,21 +1829,24 @@
       <c r="C38" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
         <v>54</v>
       </c>
-      <c r="E38">
+      <c r="G38">
         <v>25</v>
       </c>
-      <c r="F38">
+      <c r="H38">
         <v>1.1599999999999999E-2</v>
       </c>
-      <c r="G38">
-        <f xml:space="preserve"> E38*F38</f>
+      <c r="I38">
+        <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -1716,21 +1856,24 @@
       <c r="C39" t="s">
         <v>67</v>
       </c>
-      <c r="D39">
+      <c r="E39" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39">
         <v>16</v>
       </c>
-      <c r="E39">
+      <c r="G39">
         <v>30</v>
       </c>
-      <c r="F39">
+      <c r="H39">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="G39">
-        <f xml:space="preserve"> E39*F39</f>
+      <c r="I39">
+        <f t="shared" si="1"/>
         <v>0.53999999999999992</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -1740,21 +1883,24 @@
       <c r="C40" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D40">
+      <c r="E40" t="s">
+        <v>70</v>
+      </c>
+      <c r="F40">
         <v>1</v>
       </c>
-      <c r="E40">
+      <c r="G40">
         <v>10</v>
       </c>
-      <c r="F40">
+      <c r="H40">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="G40">
-        <f xml:space="preserve"> E40*F40</f>
+      <c r="I40">
+        <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -1764,21 +1910,24 @@
       <c r="C41" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D41">
+      <c r="E41" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41">
         <v>8</v>
       </c>
-      <c r="E41">
+      <c r="G41">
         <v>20</v>
       </c>
-      <c r="F41">
+      <c r="H41">
         <v>0.108</v>
       </c>
-      <c r="G41">
-        <f xml:space="preserve"> E41*F41</f>
+      <c r="I41">
+        <f t="shared" si="1"/>
         <v>2.16</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>82</v>
       </c>
@@ -1788,21 +1937,24 @@
       <c r="C42" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="9">
+      <c r="E42" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" s="9">
         <v>4</v>
       </c>
-      <c r="E42" s="9">
+      <c r="G42" s="9">
         <v>10</v>
       </c>
-      <c r="F42" s="9">
+      <c r="H42" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G42">
-        <f xml:space="preserve"> E42*F42</f>
+      <c r="I42">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -1812,21 +1964,24 @@
       <c r="C43" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D43">
+      <c r="E43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43">
         <v>4</v>
       </c>
-      <c r="E43" s="9">
+      <c r="G43" s="9">
         <v>10</v>
       </c>
-      <c r="F43">
+      <c r="H43">
         <v>0.108</v>
       </c>
-      <c r="G43">
-        <f xml:space="preserve"> E43*F43</f>
+      <c r="I43">
+        <f t="shared" si="1"/>
         <v>1.08</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -1836,21 +1991,24 @@
       <c r="C44" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D44">
+      <c r="E44" t="s">
+        <v>74</v>
+      </c>
+      <c r="F44">
         <v>4</v>
       </c>
-      <c r="E44" s="9">
+      <c r="G44" s="9">
         <v>10</v>
       </c>
-      <c r="F44">
+      <c r="H44">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="G44">
-        <f xml:space="preserve"> E44*F44</f>
+      <c r="I44">
+        <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>75</v>
       </c>
@@ -1860,51 +2018,55 @@
       <c r="C45" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D45">
+      <c r="E45" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45">
         <v>4</v>
       </c>
-      <c r="E45" s="9">
+      <c r="G45" s="9">
         <v>10</v>
       </c>
-      <c r="F45">
+      <c r="H45">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="G45">
-        <f xml:space="preserve"> E45*F45</f>
+      <c r="I45">
+        <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F47" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
         <v>113</v>
       </c>
-      <c r="G47">
-        <f xml:space="preserve"> SUM(G2:G45)</f>
+      <c r="I47">
+        <f xml:space="preserve"> SUM(I2:I45)</f>
         <v>252.16800000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F48" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
         <v>112</v>
       </c>
-      <c r="G48">
+      <c r="I48">
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F49" t="s">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
         <v>111</v>
       </c>
-      <c r="G49">
-        <f xml:space="preserve"> G47*(1+G48)</f>
+      <c r="I49">
+        <f xml:space="preserve"> I47*(1+I48)</f>
         <v>264.77640000000002</v>
-      </c>
-      <c r="H49" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added just prices bom.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donald.dunn\Documents\School\Win_18\ENEL 400\AlbatrossHardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob Dunn\Documents\School\Win_18\ENEL 400\AlbatrossHardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F739BC-22CA-403B-835B-4836EFB1FC77}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1C43A2-4CDF-492F-A326-1811D72EA2BE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="117">
   <si>
     <t>Part Number</t>
   </si>
@@ -367,6 +367,15 @@
   </si>
   <si>
     <t xml:space="preserve">Sum = </t>
+  </si>
+  <si>
+    <t>Board Stand Off</t>
+  </si>
+  <si>
+    <t>board Stand Off</t>
+  </si>
+  <si>
+    <t>RPC4731-ND</t>
   </si>
 </sst>
 </file>
@@ -415,7 +424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -428,8 +437,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -437,11 +452,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -450,19 +502,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,8 +548,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3124FECC-685F-44ED-89EB-7BB8EC99C60E}" name="Table2" displayName="Table2" ref="A1:C45" totalsRowShown="0">
-  <autoFilter ref="A1:C45" xr:uid="{26B14785-F214-412C-B38B-156AC59956A2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3124FECC-685F-44ED-89EB-7BB8EC99C60E}" name="Table2" displayName="Table2" ref="A1:C46" totalsRowShown="0">
+  <autoFilter ref="A1:C46" xr:uid="{26B14785-F214-412C-B38B-156AC59956A2}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1985A9EF-31F9-41CF-A274-0B3CC20EF885}" name="Name"/>
     <tableColumn id="2" xr3:uid="{FDABFAB7-B05C-4824-AE4F-7A63FD8E1B2E}" name="Board Referances"/>
@@ -493,8 +560,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{23991475-40B1-4CAF-90D7-8B2C9B8BC9AA}" name="Table4" displayName="Table4" ref="E1:I49" totalsRowShown="0">
-  <autoFilter ref="E1:I49" xr:uid="{6DADFDAD-0593-4B9A-BB61-05154921BBFB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{23991475-40B1-4CAF-90D7-8B2C9B8BC9AA}" name="Table4" displayName="Table4" ref="F1:J50" totalsRowShown="0">
+  <autoFilter ref="F1:J50" xr:uid="{6DADFDAD-0593-4B9A-BB61-05154921BBFB}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{99B432BE-09FD-4E1A-8A62-478D991540D5}" name="Name"/>
     <tableColumn id="2" xr3:uid="{0948B9F9-0483-4286-B335-DDDCF59F86F4}" name="# needed"/>
@@ -803,26 +870,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:I49"/>
+      <selection activeCell="F1" sqref="F1:J50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="23.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -832,23 +899,23 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -858,24 +925,24 @@
       <c r="C2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>8</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>15</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.37</v>
       </c>
-      <c r="I2">
-        <f xml:space="preserve"> G2*H2</f>
+      <c r="J2">
+        <f xml:space="preserve"> H2*I2</f>
         <v>5.55</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -885,24 +952,24 @@
       <c r="C3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>10</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>14</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.39700000000000002</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I30" si="0" xml:space="preserve"> G3*H3</f>
+      <c r="J3">
+        <f t="shared" ref="J3:J31" si="0" xml:space="preserve"> H3*I3</f>
         <v>5.5579999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -912,25 +979,25 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>4</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>6</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.48</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>2.88</v>
       </c>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -940,24 +1007,24 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>7</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>10</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.20200000000000001</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>2.02</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -967,24 +1034,24 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>5</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>10</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.218</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -994,25 +1061,25 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>4</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>7</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.43</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>3.01</v>
       </c>
-      <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1022,24 +1089,24 @@
       <c r="C8" t="s">
         <v>99</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>21</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>1</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>5</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.49</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f t="shared" si="0"/>
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1049,24 +1116,24 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>6</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>8</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1076,24 +1143,24 @@
       <c r="C10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>33</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>6</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>10</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.379</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f t="shared" si="0"/>
         <v>3.79</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1103,24 +1170,24 @@
       <c r="C11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>42</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>2</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>4</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.25</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1130,24 +1197,24 @@
       <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>44</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
       </c>
       <c r="G12">
         <v>3</v>
       </c>
       <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
         <v>0.66</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <f t="shared" si="0"/>
         <v>1.98</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1157,78 +1224,78 @@
       <c r="C13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>46</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
         <v>3.58</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>3.58</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>47</v>
       </c>
       <c r="B14" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>47</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>1</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>3</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.89</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <f t="shared" si="0"/>
         <v>2.67</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>48</v>
       </c>
       <c r="B15" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>48</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>1</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>3</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>2.06</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f t="shared" si="0"/>
         <v>6.18</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -1238,24 +1305,24 @@
       <c r="C16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>49</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
       </c>
       <c r="G16">
         <v>2</v>
       </c>
       <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
         <v>10.9</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <f t="shared" si="0"/>
         <v>21.8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1265,24 +1332,24 @@
       <c r="C17" t="s">
         <v>51</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>50</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <v>14.61</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <f t="shared" si="0"/>
         <v>14.61</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1292,24 +1359,24 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>25</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>1</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>2</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>0.39</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1319,24 +1386,24 @@
       <c r="C19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>27</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>8</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>10</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>0.54</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1346,24 +1413,24 @@
       <c r="C20" t="s">
         <v>53</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>26</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>8</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>10</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>1.599</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <f t="shared" si="0"/>
         <v>15.99</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1373,24 +1440,24 @@
       <c r="C21" t="s">
         <v>59</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>58</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>25</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>10</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>0.14899999999999999</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <f t="shared" si="0"/>
         <v>1.49</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1400,21 +1467,21 @@
       <c r="C22" t="s">
         <v>69</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>28</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1424,24 +1491,24 @@
       <c r="C23" t="s">
         <v>30</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>29</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>1</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>2</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>3.83</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <f t="shared" si="0"/>
         <v>7.66</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1451,51 +1518,51 @@
       <c r="C24" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>31</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>4</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>5</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>8.91</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <f t="shared" si="0"/>
         <v>44.55</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>32</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>14</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>15</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>0.437</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <f t="shared" si="0"/>
         <v>6.5549999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1505,51 +1572,51 @@
       <c r="C26" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>34</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>4</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>5</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>3.9</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <f t="shared" si="0"/>
         <v>19.5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>35</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>35</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>4</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>5</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>2.91</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <f t="shared" si="0"/>
         <v>14.55</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1559,24 +1626,24 @@
       <c r="C28" t="s">
         <v>37</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>36</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>4</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>5</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>3.55</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <f t="shared" si="0"/>
         <v>17.75</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1586,24 +1653,24 @@
       <c r="C29" t="s">
         <v>39</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>38</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>4</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>5</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>2.4</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1613,452 +1680,476 @@
       <c r="C30" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>55</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>1</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>2</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>2.99</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <f t="shared" si="0"/>
         <v>5.98</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31">
+        <v>4</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31">
+        <v>0.44</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C32" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F32" t="s">
         <v>40</v>
       </c>
-      <c r="F31">
+      <c r="G32">
         <v>9</v>
       </c>
-      <c r="G31">
+      <c r="H32">
         <v>15</v>
       </c>
-      <c r="H31">
+      <c r="I32">
         <v>0.159</v>
       </c>
-      <c r="I31">
-        <f t="shared" ref="I31:I45" si="1" xml:space="preserve"> G31*H31</f>
+      <c r="J32">
+        <f t="shared" ref="J32:J46" si="1" xml:space="preserve"> H32*I32</f>
         <v>2.3850000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C33" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F33" t="s">
         <v>12</v>
       </c>
-      <c r="F32">
+      <c r="G33">
         <v>1</v>
       </c>
-      <c r="G32">
+      <c r="H33">
         <v>10</v>
       </c>
-      <c r="H32">
+      <c r="I33">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="I32">
+      <c r="J33">
         <f t="shared" si="1"/>
         <v>0.74</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F34" t="s">
         <v>13</v>
       </c>
-      <c r="F33">
+      <c r="G34">
         <v>19</v>
       </c>
-      <c r="G33">
+      <c r="H34">
         <v>30</v>
       </c>
-      <c r="H33">
+      <c r="I34">
         <v>0.03</v>
       </c>
-      <c r="I33">
+      <c r="J34">
         <f t="shared" si="1"/>
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:10" ht="47.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C35" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F35" t="s">
         <v>23</v>
       </c>
-      <c r="F34">
+      <c r="G35">
         <v>2</v>
       </c>
-      <c r="G34">
+      <c r="H35">
         <v>10</v>
       </c>
-      <c r="H34">
+      <c r="I35">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="I34">
+      <c r="J35">
         <f t="shared" si="1"/>
         <v>0.84000000000000008</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C36" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F36" t="s">
         <v>24</v>
       </c>
-      <c r="F35">
+      <c r="G36">
         <v>1</v>
       </c>
-      <c r="G35">
+      <c r="H36">
         <v>10</v>
       </c>
-      <c r="H35">
+      <c r="I36">
         <v>0.10199999999999999</v>
       </c>
-      <c r="I35">
+      <c r="J36">
         <f t="shared" si="1"/>
         <v>1.02</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C37" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F37" t="s">
         <v>41</v>
       </c>
-      <c r="F36">
+      <c r="G37">
         <v>2</v>
       </c>
-      <c r="G36">
+      <c r="H37">
         <v>10</v>
       </c>
-      <c r="H36">
+      <c r="I37">
         <v>0.122</v>
       </c>
-      <c r="I36">
+      <c r="J37">
         <f t="shared" si="1"/>
         <v>1.22</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F38" t="s">
         <v>22</v>
       </c>
-      <c r="F37">
+      <c r="G38">
         <v>24</v>
       </c>
-      <c r="G37">
+      <c r="H38">
         <v>100</v>
       </c>
-      <c r="H37">
+      <c r="I38">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="I37">
+      <c r="J38">
         <f t="shared" si="1"/>
         <v>4.1000000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F39" t="s">
         <v>11</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G39" t="s">
         <v>54</v>
       </c>
-      <c r="G38">
+      <c r="H39">
         <v>25</v>
       </c>
-      <c r="H38">
+      <c r="I39">
         <v>1.1599999999999999E-2</v>
       </c>
-      <c r="I38">
+      <c r="J39">
         <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F40" t="s">
         <v>65</v>
       </c>
-      <c r="F39">
+      <c r="G40">
         <v>16</v>
       </c>
-      <c r="G39">
+      <c r="H40">
         <v>30</v>
       </c>
-      <c r="H39">
+      <c r="I40">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I39">
+      <c r="J40">
         <f t="shared" si="1"/>
         <v>0.53999999999999992</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:10" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C41" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F41" t="s">
         <v>70</v>
       </c>
-      <c r="F40">
+      <c r="G41">
         <v>1</v>
       </c>
-      <c r="G40">
+      <c r="H41">
         <v>10</v>
       </c>
-      <c r="H40">
+      <c r="I41">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I40">
+      <c r="J41">
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F42" t="s">
         <v>73</v>
       </c>
-      <c r="F41">
+      <c r="G42">
         <v>8</v>
       </c>
-      <c r="G41">
+      <c r="H42">
         <v>20</v>
       </c>
-      <c r="H41">
+      <c r="I42">
         <v>0.108</v>
       </c>
-      <c r="I41">
+      <c r="J42">
         <f t="shared" si="1"/>
         <v>2.16</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B43" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C43" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="F43" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F42" s="9">
+      <c r="G43" s="5">
         <v>4</v>
       </c>
-      <c r="G42" s="9">
+      <c r="H43" s="5">
         <v>10</v>
       </c>
-      <c r="H42" s="9">
+      <c r="I43" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I42">
+      <c r="J43">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F44" t="s">
         <v>62</v>
       </c>
-      <c r="F43">
+      <c r="G44">
         <v>4</v>
       </c>
-      <c r="G43" s="9">
+      <c r="H44" s="5">
         <v>10</v>
       </c>
-      <c r="H43">
+      <c r="I44">
         <v>0.108</v>
       </c>
-      <c r="I43">
+      <c r="J44">
         <f t="shared" si="1"/>
         <v>1.08</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F45" t="s">
         <v>74</v>
       </c>
-      <c r="F44">
+      <c r="G45">
         <v>4</v>
       </c>
-      <c r="G44" s="9">
+      <c r="H45" s="5">
         <v>10</v>
       </c>
-      <c r="H44">
+      <c r="I45">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I44">
+      <c r="J45">
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C46" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F46" t="s">
         <v>75</v>
       </c>
-      <c r="F45">
+      <c r="G46">
         <v>4</v>
       </c>
-      <c r="G45" s="9">
+      <c r="H46" s="5">
         <v>10</v>
       </c>
-      <c r="H45">
+      <c r="I46">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I45">
+      <c r="J46">
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H47" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I48" t="s">
         <v>113</v>
       </c>
-      <c r="I47">
-        <f xml:space="preserve"> SUM(I2:I45)</f>
-        <v>252.16800000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H48" t="s">
+      <c r="J48">
+        <f xml:space="preserve"> SUM(J2:J46)</f>
+        <v>254.36799999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I49" t="s">
         <v>112</v>
       </c>
-      <c r="I48">
+      <c r="J49">
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H49" t="s">
+    <row r="50" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I50" t="s">
         <v>111</v>
       </c>
-      <c r="I49">
-        <f xml:space="preserve"> I47*(1+I48)</f>
-        <v>264.77640000000002</v>
+      <c r="J50">
+        <f xml:space="preserve"> J48*(1+J49)</f>
+        <v>267.08640000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added power switch to the bom, bom excel sheet needs help.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob Dunn\Documents\School\Win_18\ENEL 400\AlbatrossHardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donald.dunn\Documents\School\Win_18\ENEL 400\AlbatrossHardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1C43A2-4CDF-492F-A326-1811D72EA2BE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98163B7-FA64-4EF4-915E-C21BDF3DA640}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="115">
   <si>
     <t>Part Number</t>
   </si>
@@ -120,18 +120,12 @@
     <t>1297-1108-1-ND</t>
   </si>
   <si>
-    <t>6pos screw term</t>
-  </si>
-  <si>
     <t>4pin vertical 2.54 head</t>
   </si>
   <si>
     <t>2.54mm 2pin male head</t>
   </si>
   <si>
-    <t>buzzer threw hole</t>
-  </si>
-  <si>
     <t>buzzer wired</t>
   </si>
   <si>
@@ -345,18 +339,12 @@
     <t>WM13209-ND</t>
   </si>
   <si>
-    <t>1297-1112-1-ND</t>
-  </si>
-  <si>
     <t>S7002-ND</t>
   </si>
   <si>
     <t>102-3740-ND</t>
   </si>
   <si>
-    <t>668-1204-ND</t>
-  </si>
-  <si>
     <t>Extended</t>
   </si>
   <si>
@@ -376,6 +364,12 @@
   </si>
   <si>
     <t>RPC4731-ND</t>
+  </si>
+  <si>
+    <t>Power Switch</t>
+  </si>
+  <si>
+    <t>1091-1013-ND</t>
   </si>
 </sst>
 </file>
@@ -493,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -505,23 +499,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -529,7 +517,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,20 +537,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3124FECC-685F-44ED-89EB-7BB8EC99C60E}" name="Table2" displayName="Table2" ref="A1:C46" totalsRowShown="0">
-  <autoFilter ref="A1:C46" xr:uid="{26B14785-F214-412C-B38B-156AC59956A2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3124FECC-685F-44ED-89EB-7BB8EC99C60E}" name="Table2" displayName="Table2" ref="A1:C47" totalsRowShown="0">
+  <autoFilter ref="A1:C47" xr:uid="{26B14785-F214-412C-B38B-156AC59956A2}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1985A9EF-31F9-41CF-A274-0B3CC20EF885}" name="Name"/>
     <tableColumn id="2" xr3:uid="{FDABFAB7-B05C-4824-AE4F-7A63FD8E1B2E}" name="Board Referances"/>
     <tableColumn id="3" xr3:uid="{87EC0948-013D-4678-BE41-F392549DECFF}" name="Part Number"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{23991475-40B1-4CAF-90D7-8B2C9B8BC9AA}" name="Table4" displayName="Table4" ref="F1:J50" totalsRowShown="0">
-  <autoFilter ref="F1:J50" xr:uid="{6DADFDAD-0593-4B9A-BB61-05154921BBFB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{23991475-40B1-4CAF-90D7-8B2C9B8BC9AA}" name="Table4" displayName="Table4" ref="F1:J51" totalsRowShown="0">
+  <autoFilter ref="F1:J51" xr:uid="{6DADFDAD-0593-4B9A-BB61-05154921BBFB}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{99B432BE-09FD-4E1A-8A62-478D991540D5}" name="Name"/>
     <tableColumn id="2" xr3:uid="{0948B9F9-0483-4286-B335-DDDCF59F86F4}" name="# needed"/>
@@ -870,26 +859,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:J50"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" customWidth="1"/>
-    <col min="6" max="6" width="23.1796875" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -912,18 +901,18 @@
         <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -942,15 +931,15 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -965,16 +954,16 @@
         <v>0.39700000000000002</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J31" si="0" xml:space="preserve"> H3*I3</f>
+        <f t="shared" ref="J3:J23" si="0" xml:space="preserve"> H3*I3</f>
         <v>5.5579999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -997,12 +986,12 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -1024,12 +1013,12 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -1051,12 +1040,12 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -1079,15 +1068,15 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F8" t="s">
         <v>21</v>
@@ -1106,12 +1095,12 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -1133,18 +1122,18 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10">
         <v>6</v>
@@ -1160,18 +1149,18 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -1187,18 +1176,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -1214,18 +1203,18 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1241,18 +1230,18 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1268,18 +1257,18 @@
         <v>2.67</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1295,18 +1284,18 @@
         <v>6.18</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -1322,18 +1311,18 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1349,15 +1338,15 @@
         <v>14.61</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s">
         <v>25</v>
@@ -1376,15 +1365,15 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
         <v>27</v>
@@ -1403,15 +1392,15 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
         <v>26</v>
@@ -1430,18 +1419,18 @@
         <v>15.99</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G21">
         <v>25</v>
@@ -1457,15 +1446,15 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F22" t="s">
         <v>28</v>
@@ -1481,12 +1470,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
@@ -1508,69 +1497,69 @@
         <v>7.66</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>106</v>
+        <v>59</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="F24" t="s">
         <v>31</v>
       </c>
       <c r="G24">
+        <v>14</v>
+      </c>
+      <c r="H24">
+        <v>15</v>
+      </c>
+      <c r="I24">
+        <v>0.437</v>
+      </c>
+      <c r="J24">
+        <f xml:space="preserve"> H24*I24</f>
+        <v>6.5549999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25">
         <v>4</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <v>5</v>
       </c>
-      <c r="I24">
-        <v>8.91</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="0"/>
-        <v>44.55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25">
-        <v>14</v>
-      </c>
-      <c r="H25">
-        <v>15</v>
-      </c>
       <c r="I25">
-        <v>0.437</v>
+        <v>2.91</v>
       </c>
       <c r="J25">
-        <f t="shared" si="0"/>
-        <v>6.5549999999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+        <f xml:space="preserve"> H25*I25</f>
+        <v>14.55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>109</v>
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
       </c>
       <c r="F26" t="s">
         <v>34</v>
@@ -1582,25 +1571,25 @@
         <v>5</v>
       </c>
       <c r="I26">
-        <v>3.9</v>
+        <v>3.55</v>
       </c>
       <c r="J26">
-        <f t="shared" si="0"/>
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+        <f xml:space="preserve"> H26*I26</f>
+        <v>17.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>108</v>
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G27">
         <v>4</v>
@@ -1609,52 +1598,49 @@
         <v>5</v>
       </c>
       <c r="I27">
-        <v>2.91</v>
+        <v>2.4</v>
       </c>
       <c r="J27">
-        <f t="shared" si="0"/>
-        <v>14.55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+        <f xml:space="preserve"> H27*I27</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" t="s">
-        <v>37</v>
+        <v>59</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="G28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I28">
-        <v>3.55</v>
+        <v>2.99</v>
       </c>
       <c r="J28">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+        <f xml:space="preserve"> H28*I28</f>
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" t="s">
-        <v>39</v>
+        <v>111</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="G29">
         <v>4</v>
@@ -1663,493 +1649,482 @@
         <v>5</v>
       </c>
       <c r="I29">
-        <v>2.4</v>
+        <v>0.44</v>
       </c>
       <c r="J29">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+        <f xml:space="preserve"> H29*I29</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>56</v>
+        <v>113</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="F30" t="s">
-        <v>55</v>
+        <v>113</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30">
-        <v>2.99</v>
+        <v>2.8</v>
       </c>
       <c r="J30">
-        <f t="shared" si="0"/>
-        <v>5.98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F31" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31">
-        <v>4</v>
-      </c>
-      <c r="H31">
-        <v>5</v>
-      </c>
-      <c r="I31">
-        <v>0.44</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G32">
+        <f xml:space="preserve"> H30*I30</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="6">
         <v>9</v>
       </c>
-      <c r="H32">
+      <c r="H31" s="6">
         <v>15</v>
       </c>
-      <c r="I32">
+      <c r="I31" s="6">
         <v>0.159</v>
       </c>
-      <c r="J32">
-        <f t="shared" ref="J32:J46" si="1" xml:space="preserve"> H32*I32</f>
+      <c r="J31" s="17">
+        <f t="shared" ref="J31:J45" si="1" xml:space="preserve"> H31*I31</f>
         <v>2.3850000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
+    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="B32" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G33">
+      <c r="G32" s="8">
         <v>1</v>
       </c>
-      <c r="H33">
+      <c r="H32" s="8">
         <v>10</v>
       </c>
-      <c r="I33">
+      <c r="I32" s="8">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J33">
+      <c r="J32" s="9">
         <f t="shared" si="1"/>
         <v>0.74</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
+    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="B33" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G34">
+      <c r="G33" s="6">
         <v>19</v>
       </c>
-      <c r="H34">
+      <c r="H33" s="6">
         <v>30</v>
       </c>
-      <c r="I34">
+      <c r="I33" s="6">
         <v>0.03</v>
       </c>
-      <c r="J34">
+      <c r="J33" s="17">
         <f t="shared" si="1"/>
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="47.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
+    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="B34" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G35">
+      <c r="G34" s="8">
         <v>2</v>
       </c>
-      <c r="H35">
+      <c r="H34" s="8">
         <v>10</v>
       </c>
-      <c r="I35">
+      <c r="I34" s="8">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="J35">
+      <c r="J34" s="9">
         <f t="shared" si="1"/>
         <v>0.84000000000000008</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="8" t="s">
+    <row r="35" spans="1:10" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="B35" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G36">
+      <c r="G35" s="6">
         <v>1</v>
       </c>
-      <c r="H36">
+      <c r="H35" s="6">
         <v>10</v>
       </c>
-      <c r="I36">
+      <c r="I35" s="6">
         <v>0.10199999999999999</v>
       </c>
-      <c r="J36">
+      <c r="J35" s="17">
         <f t="shared" si="1"/>
         <v>1.02</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="F37" t="s">
-        <v>41</v>
-      </c>
-      <c r="G37">
+    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="8">
         <v>2</v>
       </c>
-      <c r="H37">
+      <c r="H36" s="8">
         <v>10</v>
       </c>
-      <c r="I37">
+      <c r="I36" s="8">
         <v>0.122</v>
       </c>
-      <c r="J37">
+      <c r="J36" s="9">
         <f t="shared" si="1"/>
         <v>1.22</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="8" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="B37" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G38">
+      <c r="G37" s="6">
         <v>24</v>
       </c>
-      <c r="H38">
+      <c r="H37" s="6">
         <v>100</v>
       </c>
-      <c r="I38">
+      <c r="I37" s="6">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="J38">
+      <c r="J37" s="17">
         <f t="shared" si="1"/>
         <v>4.1000000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="B38" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G39" t="s">
-        <v>54</v>
-      </c>
-      <c r="H39">
+      <c r="G38" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="8">
         <v>25</v>
       </c>
-      <c r="I39">
+      <c r="I38" s="8">
         <v>1.1599999999999999E-2</v>
       </c>
-      <c r="J39">
+      <c r="J38" s="9">
         <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="8" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F40" t="s">
-        <v>65</v>
-      </c>
-      <c r="G40">
+      <c r="F39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G39" s="6">
         <v>16</v>
       </c>
-      <c r="H40">
+      <c r="H39" s="6">
         <v>30</v>
       </c>
-      <c r="I40">
+      <c r="I39" s="6">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J40">
+      <c r="J39" s="17">
         <f t="shared" si="1"/>
         <v>0.53999999999999992</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F41" t="s">
-        <v>70</v>
-      </c>
-      <c r="G41">
+      <c r="F40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G40" s="8">
         <v>1</v>
       </c>
-      <c r="H41">
+      <c r="H40" s="8">
         <v>10</v>
       </c>
-      <c r="I41">
+      <c r="I40" s="8">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J41">
+      <c r="J40" s="9">
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F42" t="s">
-        <v>73</v>
-      </c>
-      <c r="G42">
+    <row r="41" spans="1:10" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G41" s="6">
         <v>8</v>
       </c>
-      <c r="H42">
+      <c r="H41" s="6">
         <v>20</v>
       </c>
-      <c r="I42">
+      <c r="I41" s="6">
         <v>0.108</v>
       </c>
-      <c r="J42">
+      <c r="J41" s="17">
         <f t="shared" si="1"/>
         <v>2.16</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G43" s="5">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" s="15">
         <v>4</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H42" s="15">
         <v>10</v>
       </c>
-      <c r="I43" s="5">
+      <c r="I42" s="15">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J43">
+      <c r="J42" s="9">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="F44" t="s">
-        <v>62</v>
-      </c>
-      <c r="G44">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G43" s="6">
         <v>4</v>
       </c>
-      <c r="H44" s="5">
+      <c r="H43" s="15">
         <v>10</v>
       </c>
-      <c r="I44">
+      <c r="I43" s="6">
         <v>0.108</v>
       </c>
-      <c r="J44">
+      <c r="J43" s="17">
         <f t="shared" si="1"/>
         <v>1.08</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="F45" t="s">
-        <v>74</v>
-      </c>
-      <c r="G45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G44" s="8">
         <v>4</v>
       </c>
-      <c r="H45" s="5">
+      <c r="H44" s="15">
         <v>10</v>
       </c>
-      <c r="I45">
+      <c r="I44" s="8">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J45">
+      <c r="J44" s="9">
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A46" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="F46" t="s">
-        <v>75</v>
-      </c>
-      <c r="G46">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45" s="6">
         <v>4</v>
       </c>
-      <c r="H46" s="5">
+      <c r="H45" s="15">
         <v>10</v>
       </c>
-      <c r="I46">
+      <c r="I45" s="6">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J46">
+      <c r="J45" s="17">
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I48" t="s">
-        <v>113</v>
-      </c>
-      <c r="J48">
-        <f xml:space="preserve"> SUM(J2:J46)</f>
-        <v>254.36799999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I49" t="s">
-        <v>112</v>
-      </c>
-      <c r="J49">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F46" s="7"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="9"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F47" s="5"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J47" s="17">
+        <f xml:space="preserve"> SUM(J2:J45)</f>
+        <v>193.11800000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F48" s="7"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J48" s="9">
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I50" t="s">
-        <v>111</v>
-      </c>
-      <c r="J50">
-        <f xml:space="preserve"> J48*(1+J49)</f>
-        <v>267.08640000000003</v>
+    <row r="49" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="5"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J49" s="17">
+        <f xml:space="preserve"> J47*(1+J48)</f>
+        <v>202.77390000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>